<commit_message>
final commit on 18-Jul-2020
</commit_message>
<xml_diff>
--- a/resource/testdata.xlsx
+++ b/resource/testdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUNILBHATRA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SDET Workspace_03-Jun-2020\SeleniumElearningDemoProject\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313F3F8B-91A2-4514-9D5C-D6DF14E35730}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42027D3-1316-4482-AC01-C829EE31D5A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>first name</t>
   </si>
@@ -48,35 +48,74 @@
     <t>phone</t>
   </si>
   <si>
-    <t>Language</t>
-  </si>
-  <si>
     <t>one</t>
   </si>
   <si>
     <t>one@one.com</t>
   </si>
   <si>
-    <t>one8</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
-    <t>one9</t>
-  </si>
-  <si>
-    <t>one10</t>
+    <t>language</t>
+  </si>
+  <si>
+    <t>validation</t>
+  </si>
+  <si>
+    <t>first101</t>
+  </si>
+  <si>
+    <t>last201</t>
+  </si>
+  <si>
+    <t>An e-mail has been sent to remind you of your login and password.</t>
+  </si>
+  <si>
+    <t>one1001</t>
+  </si>
+  <si>
+    <t>one1002</t>
+  </si>
+  <si>
+    <t>one1003</t>
+  </si>
+  <si>
+    <t>one1004</t>
+  </si>
+  <si>
+    <t>first102</t>
+  </si>
+  <si>
+    <t>first103</t>
+  </si>
+  <si>
+    <t>first104</t>
+  </si>
+  <si>
+    <t>last202</t>
+  </si>
+  <si>
+    <t>last203</t>
+  </si>
+  <si>
+    <t>last204</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -384,20 +423,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="57.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,88 +465,130 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2">
         <v>123</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3">
         <v>123</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4">
         <v>123</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>123</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
incorporated driver and remove xpath
</commit_message>
<xml_diff>
--- a/resource/testdata.xlsx
+++ b/resource/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SDET Workspace_03-Jun-2020\SeleniumElearningDemoProject\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42027D3-1316-4482-AC01-C829EE31D5A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6619965-1ABB-455D-96A3-3E3DA43E294C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,6 +72,24 @@
     <t>An e-mail has been sent to remind you of your login and password.</t>
   </si>
   <si>
+    <t>first102</t>
+  </si>
+  <si>
+    <t>first103</t>
+  </si>
+  <si>
+    <t>first104</t>
+  </si>
+  <si>
+    <t>last202</t>
+  </si>
+  <si>
+    <t>last203</t>
+  </si>
+  <si>
+    <t>last204</t>
+  </si>
+  <si>
     <t>one1001</t>
   </si>
   <si>
@@ -82,24 +100,6 @@
   </si>
   <si>
     <t>one1004</t>
-  </si>
-  <si>
-    <t>first102</t>
-  </si>
-  <si>
-    <t>first103</t>
-  </si>
-  <si>
-    <t>first104</t>
-  </si>
-  <si>
-    <t>last202</t>
-  </si>
-  <si>
-    <t>last203</t>
-  </si>
-  <si>
-    <t>last204</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,7 +482,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -502,16 +502,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -531,16 +531,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -560,16 +560,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>

</xml_diff>